<commit_message>
add moment trade strategy & sort common module
</commit_message>
<xml_diff>
--- a/doc/数字货币/主流币种.xlsx
+++ b/doc/数字货币/主流币种.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24045" windowHeight="12525"/>
+    <workbookView windowWidth="29868" windowHeight="13380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="主流币种分类汇总" sheetId="1" r:id="rId1"/>
+    <sheet name="主流币种" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,9 +28,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
-    <t>类别</t>
+    <t>名字</t>
   </si>
   <si>
     <t>特点</t>
@@ -72,21 +73,19 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="5"/>
-        <rFont val="宋体"/>
+        <rFont val="Microsoft YaHei"/>
         <charset val="134"/>
-        <scheme val="minor"/>
       </rPr>
       <t>没有真实的技术团队在按照白皮书进行开发维护</t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Microsoft YaHei"/>
         <charset val="134"/>
-        <scheme val="minor"/>
       </rPr>
       <t>，只以发币圈钱为目的</t>
     </r>
@@ -106,6 +105,9 @@
 3.承诺单边上扬只涨不跌 
 拉人进场，有丰厚的佣金回报。</t>
   </si>
+  <si>
+    <t>所处链</t>
+  </si>
 </sst>
 </file>
 
@@ -117,7 +119,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,18 +129,31 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Microsoft YaHei"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Microsoft YaHei"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Microsoft YaHei"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="10.5"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10.5"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -283,11 +298,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="5"/>
-      <name val="宋体"/>
+      <name val="Microsoft YaHei"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -610,150 +624,159 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1283,70 +1306,158 @@
   <sheetPr/>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="B20 D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="72.375" customWidth="1"/>
-    <col min="3" max="3" width="23.625" customWidth="1"/>
+    <col min="1" max="1" width="10.5648148148148" customWidth="1"/>
+    <col min="2" max="2" width="50.7777777777778" customWidth="1"/>
+    <col min="3" max="3" width="14.2685185185185" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" ht="22.5" customHeight="1" spans="1:3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" ht="40.5" spans="1:3">
-      <c r="A2" s="1" t="s">
+    <row r="2" ht="55.5" customHeight="1" spans="1:3">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" ht="81" spans="1:3">
-      <c r="A3" s="1" t="s">
+    <row r="3" ht="88.5" customHeight="1" spans="1:3">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" ht="40.5" spans="1:3">
-      <c r="A4" t="s">
+    <row r="4" ht="55.5" customHeight="1" spans="1:3">
+      <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" ht="120" customHeight="1" spans="1:2">
-      <c r="A5" t="s">
+    <row r="5" ht="138" customHeight="1" spans="1:3">
+      <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="2:2">
-      <c r="B6" s="4"/>
+      <c r="B6" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="10.5648148148148" customWidth="1"/>
+    <col min="2" max="2" width="11.1203703703704" customWidth="1"/>
+    <col min="3" max="3" width="50.7777777777778" customWidth="1"/>
+    <col min="4" max="4" width="14.2685185185185" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="22.5" customHeight="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" ht="55.5" customHeight="1" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" ht="88.5" customHeight="1" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" ht="55.5" customHeight="1" spans="1:4">
+      <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" ht="138" customHeight="1" spans="1:4">
+      <c r="A5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" customFormat="1" spans="3:3">
+      <c r="C6" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>